<commit_message>
Created new matlab file for newly changed comments code
</commit_message>
<xml_diff>
--- a/code/experiment/Run_1.xlsx
+++ b/code/experiment/Run_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahabdou/Documents/Interocular-grouping-and-motion/code/experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE6C4DC-7996-DC44-A854-E71DED658CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C5B2A6-45C1-3945-B0E3-353E6C16D59A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="9960" windowWidth="28040" windowHeight="17440" xr2:uid="{6B88140D-DF39-2E4A-B3E4-DA0EF96A1915}"/>
+    <workbookView xWindow="6800" yWindow="5080" windowWidth="28040" windowHeight="17440" xr2:uid="{6B88140D-DF39-2E4A-B3E4-DA0EF96A1915}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Trial</t>
   </si>
@@ -51,12 +51,6 @@
   </si>
   <si>
     <t>Color2</t>
-  </si>
-  <si>
-    <t>Orientation1</t>
-  </si>
-  <si>
-    <t>Orientation2</t>
   </si>
   <si>
     <t>red</t>
@@ -421,19 +415,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E38F54D-6D22-974E-A446-7DBA143D65FF}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="37.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,14 +444,8 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -472,14 +461,8 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -490,19 +473,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -518,14 +495,8 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -536,16 +507,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Recent changes to color code
</commit_message>
<xml_diff>
--- a/code/experiment/Run_1.xlsx
+++ b/code/experiment/Run_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahabdou/Documents/Interocular-grouping-and-motion/code/experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C5B2A6-45C1-3945-B0E3-353E6C16D59A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F19E96-0040-564C-91AD-7B7B85AE252C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6800" yWindow="5080" windowWidth="28040" windowHeight="17440" xr2:uid="{6B88140D-DF39-2E4A-B3E4-DA0EF96A1915}"/>
+    <workbookView xWindow="6800" yWindow="4920" windowWidth="28040" windowHeight="17440" xr2:uid="{6B88140D-DF39-2E4A-B3E4-DA0EF96A1915}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Trial</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>green</t>
+  </si>
+  <si>
+    <t>black</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,11 +458,11 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -489,11 +492,11 @@
       <c r="C4">
         <v>-1</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>